<commit_message>
Updated ROI history xlsx data. Added InflationRate
</commit_message>
<xml_diff>
--- a/src/NinthBall.Core/Data/ROI-History.xlsx
+++ b/src/NinthBall.Core/Data/ROI-History.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\POCs\HelloMonteCarlo\src\HelloMonteCarlo\DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\ninth-ball\src\NinthBall.Core\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F9C577-5579-4F49-8191-0D8069337A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FBD6AE-4ACB-4060-9CCC-C2DB95BD4364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{E1C51C66-5FE7-4317-BF3B-425E212419EB}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,15 +36,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Year</t>
   </si>
   <si>
-    <t>Stock</t>
+    <t>InflationRate</t>
   </si>
   <si>
-    <t>Bond</t>
+    <t>StocksROI</t>
+  </si>
+  <si>
+    <t>BondsROI</t>
   </si>
 </sst>
 </file>
@@ -431,26 +434,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C893099F-9C5C-483F-8AE8-113FCC20E12B}">
-  <dimension ref="A1:C98"/>
+  <dimension ref="A1:D98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="4" width="11.58203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1928</v>
       </c>
@@ -460,8 +469,11 @@
       <c r="C2">
         <v>8.3999999999999995E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2">
+        <v>-1.15607E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>1929</v>
       </c>
@@ -471,8 +483,11 @@
       <c r="C3">
         <v>4.2000000000000003E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3">
+        <v>5.8479999999999999E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>1930</v>
       </c>
@@ -482,8 +497,11 @@
       <c r="C4">
         <v>4.5400000000000003E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4">
+        <v>-6.3953499999999996E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>1931</v>
       </c>
@@ -493,8 +511,11 @@
       <c r="C5">
         <v>-2.5600000000000001E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5">
+        <v>-9.3167700000000006E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>1932</v>
       </c>
@@ -504,8 +525,11 @@
       <c r="C6">
         <v>8.7900000000000006E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6">
+        <v>-0.1027397</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>1933</v>
       </c>
@@ -515,8 +539,11 @@
       <c r="C7">
         <v>1.8599999999999998E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7">
+        <v>7.6336000000000008E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>1934</v>
       </c>
@@ -526,8 +553,11 @@
       <c r="C8">
         <v>7.9600000000000004E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8">
+        <v>1.51515E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>1935</v>
       </c>
@@ -537,8 +567,11 @@
       <c r="C9">
         <v>4.4699999999999997E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9">
+        <v>2.9850699999999997E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>1936</v>
       </c>
@@ -548,8 +581,11 @@
       <c r="C10">
         <v>5.0200000000000002E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10">
+        <v>1.4492799999999998E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>1937</v>
       </c>
@@ -559,8 +595,11 @@
       <c r="C11">
         <v>1.38E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11">
+        <v>2.8571399999999997E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>1938</v>
       </c>
@@ -570,8 +609,11 @@
       <c r="C12">
         <v>4.2099999999999999E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12">
+        <v>-2.7777799999999998E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>1939</v>
       </c>
@@ -581,8 +623,11 @@
       <c r="C13">
         <v>4.41E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>1940</v>
       </c>
@@ -592,8 +637,11 @@
       <c r="C14">
         <v>5.3999999999999999E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14">
+        <v>7.1428999999999998E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>1941</v>
       </c>
@@ -603,8 +651,11 @@
       <c r="C15">
         <v>-2.0199999999999999E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15">
+        <v>9.9290800000000012E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>1942</v>
       </c>
@@ -614,8 +665,11 @@
       <c r="C16">
         <v>2.29E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16">
+        <v>9.0322600000000003E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>1943</v>
       </c>
@@ -625,8 +679,11 @@
       <c r="C17">
         <v>2.4899999999999999E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17">
+        <v>2.9585799999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>1944</v>
       </c>
@@ -636,8 +693,11 @@
       <c r="C18">
         <v>2.58E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18">
+        <v>2.2988499999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>1945</v>
       </c>
@@ -647,8 +707,11 @@
       <c r="C19">
         <v>3.7999999999999999E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19">
+        <v>2.24719E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>1946</v>
       </c>
@@ -658,8 +721,11 @@
       <c r="C20">
         <v>3.1300000000000001E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20">
+        <v>0.1813187</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>1947</v>
       </c>
@@ -669,8 +735,11 @@
       <c r="C21">
         <v>9.1999999999999998E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21">
+        <v>8.8372100000000009E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>1948</v>
       </c>
@@ -680,8 +749,11 @@
       <c r="C22">
         <v>1.95E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22">
+        <v>2.99145E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>1949</v>
       </c>
@@ -691,8 +763,11 @@
       <c r="C23">
         <v>4.6600000000000003E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23">
+        <v>-2.0746899999999999E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>1950</v>
       </c>
@@ -702,8 +777,11 @@
       <c r="C24">
         <v>4.3E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="D24">
+        <v>5.9322E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>1951</v>
       </c>
@@ -713,8 +791,11 @@
       <c r="C25">
         <v>-3.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="D25">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>1952</v>
       </c>
@@ -724,8 +805,11 @@
       <c r="C26">
         <v>2.2700000000000001E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="D26">
+        <v>7.5471999999999996E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>1953</v>
       </c>
@@ -735,8 +819,11 @@
       <c r="C27">
         <v>4.1399999999999999E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="D27">
+        <v>7.4905999999999992E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>1954</v>
       </c>
@@ -746,8 +833,11 @@
       <c r="C28">
         <v>3.2899999999999999E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="D28">
+        <v>-7.4348999999999995E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>1955</v>
       </c>
@@ -757,8 +847,11 @@
       <c r="C29">
         <v>-1.34E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="D29">
+        <v>3.7452999999999996E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>1956</v>
       </c>
@@ -768,8 +861,11 @@
       <c r="C30">
         <v>-2.2599999999999999E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="D30">
+        <v>2.9850699999999997E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>1957</v>
       </c>
@@ -779,8 +875,11 @@
       <c r="C31">
         <v>6.8000000000000005E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="D31">
+        <v>2.8985500000000001E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>1958</v>
       </c>
@@ -790,8 +889,11 @@
       <c r="C32">
         <v>-2.1000000000000001E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="D32">
+        <v>1.7605599999999999E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>1959</v>
       </c>
@@ -801,8 +903,11 @@
       <c r="C33">
         <v>-2.6499999999999999E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="D33">
+        <v>1.7301E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>1960</v>
       </c>
@@ -812,8 +917,11 @@
       <c r="C34">
         <v>0.1164</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="D34">
+        <v>1.36054E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35">
         <v>1961</v>
       </c>
@@ -823,8 +931,11 @@
       <c r="C35">
         <v>2.06E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="D35">
+        <v>6.7113999999999993E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36">
         <v>1962</v>
       </c>
@@ -834,8 +945,11 @@
       <c r="C36">
         <v>5.6899999999999999E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="D36">
+        <v>1.3333299999999999E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37">
         <v>1963</v>
       </c>
@@ -845,8 +959,11 @@
       <c r="C37">
         <v>1.6799999999999999E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="D37">
+        <v>1.6447400000000001E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38">
         <v>1964</v>
       </c>
@@ -856,8 +973,11 @@
       <c r="C38">
         <v>3.73E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="D38">
+        <v>9.7087000000000007E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39">
         <v>1965</v>
       </c>
@@ -867,8 +987,11 @@
       <c r="C39">
         <v>7.1999999999999998E-3</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
+      <c r="D39">
+        <v>1.9230799999999999E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40">
         <v>1966</v>
       </c>
@@ -878,8 +1001,11 @@
       <c r="C40">
         <v>2.9100000000000001E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="D40">
+        <v>3.4591200000000003E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41">
         <v>1967</v>
       </c>
@@ -889,8 +1015,11 @@
       <c r="C41">
         <v>-1.5800000000000002E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="D41">
+        <v>3.0395099999999998E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42">
         <v>1968</v>
       </c>
@@ -900,8 +1029,11 @@
       <c r="C42">
         <v>3.27E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="D42">
+        <v>4.7197599999999999E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43">
         <v>1969</v>
       </c>
@@ -911,8 +1043,11 @@
       <c r="C43">
         <v>-5.0099999999999999E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="D43">
+        <v>6.19718E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44">
         <v>1970</v>
       </c>
@@ -922,8 +1057,11 @@
       <c r="C44">
         <v>0.16750000000000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="D44">
+        <v>5.57029E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45">
         <v>1971</v>
       </c>
@@ -933,8 +1071,11 @@
       <c r="C45">
         <v>9.7900000000000001E-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="D45">
+        <v>3.2663299999999999E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46">
         <v>1972</v>
       </c>
@@ -944,8 +1085,11 @@
       <c r="C46">
         <v>2.8199999999999999E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="D46">
+        <v>3.4063299999999998E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47">
         <v>1973</v>
       </c>
@@ -955,8 +1099,11 @@
       <c r="C47">
         <v>3.6600000000000001E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="D47">
+        <v>8.7058800000000006E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48">
         <v>1974</v>
       </c>
@@ -966,8 +1113,11 @@
       <c r="C48">
         <v>1.9900000000000001E-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
+      <c r="D48">
+        <v>0.1233766</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49">
         <v>1975</v>
       </c>
@@ -977,8 +1127,11 @@
       <c r="C49">
         <v>3.61E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:3">
+      <c r="D49">
+        <v>6.9364200000000001E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50">
         <v>1976</v>
       </c>
@@ -988,8 +1141,11 @@
       <c r="C50">
         <v>0.1598</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
+      <c r="D50">
+        <v>4.86486E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51">
         <v>1977</v>
       </c>
@@ -999,8 +1155,11 @@
       <c r="C51">
         <v>1.29E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:3">
+      <c r="D51">
+        <v>6.7010300000000009E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52">
         <v>1978</v>
       </c>
@@ -1010,8 +1169,11 @@
       <c r="C52">
         <v>-7.7999999999999996E-3</v>
       </c>
-    </row>
-    <row r="53" spans="1:3">
+      <c r="D52">
+        <v>9.0177099999999996E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53">
         <v>1979</v>
       </c>
@@ -1021,8 +1183,11 @@
       <c r="C53">
         <v>6.7000000000000002E-3</v>
       </c>
-    </row>
-    <row r="54" spans="1:3">
+      <c r="D53">
+        <v>0.13293939999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54">
         <v>1980</v>
       </c>
@@ -1032,8 +1197,11 @@
       <c r="C54">
         <v>-2.9899999999999999E-2</v>
       </c>
-    </row>
-    <row r="55" spans="1:3">
+      <c r="D54">
+        <v>0.125163</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55">
         <v>1981</v>
       </c>
@@ -1043,8 +1211,11 @@
       <c r="C55">
         <v>8.2000000000000003E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:3">
+      <c r="D55">
+        <v>8.92236E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56">
         <v>1982</v>
       </c>
@@ -1054,8 +1225,11 @@
       <c r="C56">
         <v>0.3281</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
+      <c r="D56">
+        <v>3.8297900000000003E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57">
         <v>1983</v>
       </c>
@@ -1065,8 +1239,11 @@
       <c r="C57">
         <v>3.2000000000000001E-2</v>
       </c>
-    </row>
-    <row r="58" spans="1:3">
+      <c r="D57">
+        <v>3.79098E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58">
         <v>1984</v>
       </c>
@@ -1076,8 +1253,11 @@
       <c r="C58">
         <v>0.13730000000000001</v>
       </c>
-    </row>
-    <row r="59" spans="1:3">
+      <c r="D58">
+        <v>3.94867E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59">
         <v>1985</v>
       </c>
@@ -1087,8 +1267,11 @@
       <c r="C59">
         <v>0.2571</v>
       </c>
-    </row>
-    <row r="60" spans="1:3">
+      <c r="D59">
+        <v>3.7986699999999998E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60">
         <v>1986</v>
       </c>
@@ -1098,8 +1281,11 @@
       <c r="C60">
         <v>0.24279999999999999</v>
       </c>
-    </row>
-    <row r="61" spans="1:3">
+      <c r="D60">
+        <v>1.0979000000000001E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61">
         <v>1987</v>
       </c>
@@ -1109,8 +1295,11 @@
       <c r="C61">
         <v>-4.9599999999999998E-2</v>
       </c>
-    </row>
-    <row r="62" spans="1:3">
+      <c r="D61">
+        <v>4.4343899999999999E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62">
         <v>1988</v>
       </c>
@@ -1120,8 +1309,11 @@
       <c r="C62">
         <v>8.2199999999999995E-2</v>
       </c>
-    </row>
-    <row r="63" spans="1:3">
+      <c r="D62">
+        <v>4.41941E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63">
         <v>1989</v>
       </c>
@@ -1131,8 +1323,11 @@
       <c r="C63">
         <v>0.1769</v>
       </c>
-    </row>
-    <row r="64" spans="1:3">
+      <c r="D63">
+        <v>4.6473000000000007E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64">
         <v>1990</v>
       </c>
@@ -1142,8 +1337,11 @@
       <c r="C64">
         <v>6.2399999999999997E-2</v>
       </c>
-    </row>
-    <row r="65" spans="1:3">
+      <c r="D64">
+        <v>6.1062599999999995E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65">
         <v>1991</v>
       </c>
@@ -1153,8 +1351,11 @@
       <c r="C65">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="66" spans="1:3">
+      <c r="D65">
+        <v>3.0642800000000001E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66">
         <v>1992</v>
       </c>
@@ -1164,8 +1365,11 @@
       <c r="C66">
         <v>9.3600000000000003E-2</v>
       </c>
-    </row>
-    <row r="67" spans="1:3">
+      <c r="D66">
+        <v>2.9006500000000001E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67">
         <v>1993</v>
       </c>
@@ -1175,8 +1379,11 @@
       <c r="C67">
         <v>0.1421</v>
       </c>
-    </row>
-    <row r="68" spans="1:3">
+      <c r="D67">
+        <v>2.7484099999999997E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68">
         <v>1994</v>
       </c>
@@ -1186,8 +1393,11 @@
       <c r="C68">
         <v>-8.0399999999999999E-2</v>
       </c>
-    </row>
-    <row r="69" spans="1:3">
+      <c r="D68">
+        <v>2.6749000000000002E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69">
         <v>1995</v>
       </c>
@@ -1197,8 +1407,11 @@
       <c r="C69">
         <v>0.23480000000000001</v>
       </c>
-    </row>
-    <row r="70" spans="1:3">
+      <c r="D69">
+        <v>2.53841E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70">
         <v>1996</v>
       </c>
@@ -1208,8 +1421,11 @@
       <c r="C70">
         <v>1.43E-2</v>
       </c>
-    </row>
-    <row r="71" spans="1:3">
+      <c r="D70">
+        <v>3.3224799999999999E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71">
         <v>1997</v>
       </c>
@@ -1219,8 +1435,11 @@
       <c r="C71">
         <v>9.9400000000000002E-2</v>
       </c>
-    </row>
-    <row r="72" spans="1:3">
+      <c r="D71">
+        <v>1.7023999999999997E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72">
         <v>1998</v>
       </c>
@@ -1230,8 +1449,11 @@
       <c r="C72">
         <v>0.1492</v>
       </c>
-    </row>
-    <row r="73" spans="1:3">
+      <c r="D72">
+        <v>1.6119000000000001E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73">
         <v>1999</v>
       </c>
@@ -1241,8 +1463,11 @@
       <c r="C73">
         <v>-8.2500000000000004E-2</v>
       </c>
-    </row>
-    <row r="74" spans="1:3">
+      <c r="D73">
+        <v>2.6845599999999997E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74">
         <v>2000</v>
       </c>
@@ -1252,8 +1477,11 @@
       <c r="C74">
         <v>0.1666</v>
       </c>
-    </row>
-    <row r="75" spans="1:3">
+      <c r="D74">
+        <v>3.3868099999999998E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75">
         <v>2001</v>
       </c>
@@ -1263,8 +1491,11 @@
       <c r="C75">
         <v>5.57E-2</v>
       </c>
-    </row>
-    <row r="76" spans="1:3">
+      <c r="D75">
+        <v>1.55172E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76">
         <v>2002</v>
       </c>
@@ -1274,8 +1505,11 @@
       <c r="C76">
         <v>0.1512</v>
       </c>
-    </row>
-    <row r="77" spans="1:3">
+      <c r="D76">
+        <v>2.3769100000000001E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77">
         <v>2003</v>
       </c>
@@ -1285,8 +1519,11 @@
       <c r="C77">
         <v>3.8E-3</v>
       </c>
-    </row>
-    <row r="78" spans="1:3">
+      <c r="D77">
+        <v>1.87949E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78">
         <v>2004</v>
       </c>
@@ -1296,8 +1533,11 @@
       <c r="C78">
         <v>4.4900000000000002E-2</v>
       </c>
-    </row>
-    <row r="79" spans="1:3">
+      <c r="D78">
+        <v>3.2555599999999997E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79">
         <v>2005</v>
       </c>
@@ -1307,8 +1547,11 @@
       <c r="C79">
         <v>2.87E-2</v>
       </c>
-    </row>
-    <row r="80" spans="1:3">
+      <c r="D79">
+        <v>3.4156600000000002E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80">
         <v>2006</v>
       </c>
@@ -1318,8 +1561,11 @@
       <c r="C80">
         <v>1.9599999999999999E-2</v>
       </c>
-    </row>
-    <row r="81" spans="1:3">
+      <c r="D80">
+        <v>2.5406499999999999E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
       <c r="A81">
         <v>2007</v>
       </c>
@@ -1329,8 +1575,11 @@
       <c r="C81">
         <v>0.1021</v>
       </c>
-    </row>
-    <row r="82" spans="1:3">
+      <c r="D81">
+        <v>4.08127E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
       <c r="A82">
         <v>2008</v>
       </c>
@@ -1340,8 +1589,11 @@
       <c r="C82">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="83" spans="1:3">
+      <c r="D82">
+        <v>9.1410000000000005E-4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83">
         <v>2009</v>
       </c>
@@ -1351,8 +1603,11 @@
       <c r="C83">
         <v>-0.11119999999999999</v>
       </c>
-    </row>
-    <row r="84" spans="1:3">
+      <c r="D83">
+        <v>2.7213299999999999E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
       <c r="A84">
         <v>2010</v>
       </c>
@@ -1362,8 +1617,11 @@
       <c r="C84">
         <v>8.4599999999999995E-2</v>
       </c>
-    </row>
-    <row r="85" spans="1:3">
+      <c r="D84">
+        <v>1.4957199999999999E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
       <c r="A85">
         <v>2011</v>
       </c>
@@ -1373,8 +1631,11 @@
       <c r="C85">
         <v>0.16039999999999999</v>
       </c>
-    </row>
-    <row r="86" spans="1:3">
+      <c r="D85">
+        <v>2.96242E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
       <c r="A86">
         <v>2012</v>
       </c>
@@ -1384,8 +1645,11 @@
       <c r="C86">
         <v>2.9700000000000001E-2</v>
       </c>
-    </row>
-    <row r="87" spans="1:3">
+      <c r="D86">
+        <v>1.7410200000000001E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
       <c r="A87">
         <v>2013</v>
       </c>
@@ -1395,8 +1659,11 @@
       <c r="C87">
         <v>-9.0999999999999998E-2</v>
       </c>
-    </row>
-    <row r="88" spans="1:3">
+      <c r="D87">
+        <v>1.50174E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
       <c r="A88">
         <v>2014</v>
       </c>
@@ -1406,8 +1673,11 @@
       <c r="C88">
         <v>0.1075</v>
       </c>
-    </row>
-    <row r="89" spans="1:3">
+      <c r="D88">
+        <v>7.5649000000000003E-3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
       <c r="A89">
         <v>2015</v>
       </c>
@@ -1417,8 +1687,11 @@
       <c r="C89">
         <v>1.2800000000000001E-2</v>
       </c>
-    </row>
-    <row r="90" spans="1:3">
+      <c r="D89">
+        <v>7.2951999999999991E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
       <c r="A90">
         <v>2016</v>
       </c>
@@ -1428,8 +1701,11 @@
       <c r="C90">
         <v>6.8999999999999999E-3</v>
       </c>
-    </row>
-    <row r="91" spans="1:3">
+      <c r="D90">
+        <v>2.0746199999999999E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
       <c r="A91">
         <v>2017</v>
       </c>
@@ -1439,8 +1715,11 @@
       <c r="C91">
         <v>2.8000000000000001E-2</v>
       </c>
-    </row>
-    <row r="92" spans="1:3">
+      <c r="D91">
+        <v>2.10908E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
       <c r="A92">
         <v>2018</v>
       </c>
@@ -1450,8 +1729,11 @@
       <c r="C92">
         <v>-2.0000000000000001E-4</v>
       </c>
-    </row>
-    <row r="93" spans="1:3">
+      <c r="D92">
+        <v>1.91016E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
       <c r="A93">
         <v>2019</v>
       </c>
@@ -1461,8 +1743,11 @@
       <c r="C93">
         <v>9.64E-2</v>
       </c>
-    </row>
-    <row r="94" spans="1:3">
+      <c r="D93">
+        <v>2.2851300000000001E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
       <c r="A94">
         <v>2020</v>
       </c>
@@ -1472,8 +1757,11 @@
       <c r="C94">
         <v>0.1133</v>
       </c>
-    </row>
-    <row r="95" spans="1:3">
+      <c r="D94">
+        <v>1.36201E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
       <c r="A95">
         <v>2021</v>
       </c>
@@ -1483,8 +1771,11 @@
       <c r="C95">
         <v>-4.4200000000000003E-2</v>
       </c>
-    </row>
-    <row r="96" spans="1:3">
+      <c r="D95">
+        <v>7.036400000000001E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
       <c r="A96">
         <v>2022</v>
       </c>
@@ -1494,8 +1785,11 @@
       <c r="C96">
         <v>-0.17829999999999999</v>
       </c>
-    </row>
-    <row r="97" spans="1:3">
+      <c r="D96">
+        <v>6.454399999999999E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
       <c r="A97">
         <v>2023</v>
       </c>
@@ -1505,8 +1799,11 @@
       <c r="C97">
         <v>3.8800000000000001E-2</v>
       </c>
-    </row>
-    <row r="98" spans="1:3">
+      <c r="D97">
+        <v>3.3521200000000001E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
       <c r="A98">
         <v>2024</v>
       </c>
@@ -1515,6 +1812,9 @@
       </c>
       <c r="C98">
         <v>-1.6400000000000001E-2</v>
+      </c>
+      <c r="D98">
+        <v>2.75E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>